<commit_message>
Added profile, student details
</commit_message>
<xml_diff>
--- a/attendance_report.xlsx
+++ b/attendance_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,189 +463,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>5M5</t>
+          <t>5Q1</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>LEKHYASREE MARRI</t>
+          <t>LEKHA</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>22:50</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2025-03-16</t>
+          <t>2025-03-18</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>OOPJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>5M5</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>LEKHYASREE MARRI</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>19:33</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>BEEE</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>5M5</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>LEKHYASREE MARRI</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>19:36</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>PSC</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>501</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>RANVEER SINGH</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>19:41</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>PSC</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5M5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>LEKHYASREE MARRI</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>20:30</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>OOPJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>5M5</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>LEKHYASREE MARRI</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>20:34</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>OOPJ</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>5M5</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>LEKHYASREE MARRI</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>20:35</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>2025-03-16</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>OOPJ</t>
+          <t>OOPS</t>
         </is>
       </c>
     </row>

</xml_diff>